<commit_message>
Importer: add option to import images and general improvements
- Fix importer to import stocks correctly
- Fix base importer resolve objects method by checking fields existence before querying them
- Avoid error 500 when importer goes wrong
- Add special column `ignore` that flags rows to be ignored
- Add option to provide a helper template for every importer. The template is rendered in admin when selecting the importer.

Refs POS-2493
</commit_message>
<xml_diff>
--- a/shuup/default_importer/samples/person_contact_sample.xlsx
+++ b/shuup/default_importer/samples/person_contact_sample.xlsx
@@ -256,22 +256,22 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -300,7 +300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
@@ -329,7 +329,7 @@
         <v>1123555111</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>16</v>
       </c>

</xml_diff>